<commit_message>
Realitzat canvis per pujar de nota
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innovalaus-my.sharepoint.com/personal/jordi_innovalaus_com/Documents/I+D/Proves i documentació varia/Carla proves/UiPath Workflows/Calculate Client Security Hash/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{4DBDD912-376B-4FA7-AD0A-24274EEDD007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{224F3184-32F7-46D0-845F-B1C97ECBACE5}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{4DBDD912-376B-4FA7-AD0A-24274EEDD007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46BF6548-8793-4B12-84AC-1BA178664E7F}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -284,10 +284,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,7 +586,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>